<commit_message>
add VS3 model 1
</commit_message>
<xml_diff>
--- a/derivatives/palm_data/data/ISTART_Brain2x2_110322_jbw.xlsx
+++ b/derivatives/palm_data/data/ISTART_Brain2x2_110322_jbw.xlsx
@@ -5,22 +5,23 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/Documents_Air/GitHub/istart-socdoors/derivatives/palm_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B49087D4-82D9-9F4E-AD60-3DFA65514B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E77C6154-7FE5-2A4B-B7D5-BBD8BF19B935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="620" windowWidth="26360" windowHeight="15740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ISTART_Brain2x2_110322_jbw_new" sheetId="1" r:id="rId1"/>
     <sheet name="act model 1" sheetId="2" r:id="rId2"/>
-    <sheet name="act_model_3_VS_3" sheetId="8" r:id="rId3"/>
-    <sheet name="act model 2" sheetId="3" r:id="rId4"/>
-    <sheet name="act model 3" sheetId="4" r:id="rId5"/>
-    <sheet name="ppi model 1" sheetId="5" r:id="rId6"/>
-    <sheet name="ppi model 2" sheetId="6" r:id="rId7"/>
-    <sheet name="ppi model 3" sheetId="7" r:id="rId8"/>
+    <sheet name="act_model_1_VS_3" sheetId="9" r:id="rId3"/>
+    <sheet name="act_model_3_VS_3" sheetId="8" r:id="rId4"/>
+    <sheet name="act model 2" sheetId="3" r:id="rId5"/>
+    <sheet name="act model 3" sheetId="4" r:id="rId6"/>
+    <sheet name="ppi model 1" sheetId="5" r:id="rId7"/>
+    <sheet name="ppi model 2" sheetId="6" r:id="rId8"/>
+    <sheet name="ppi model 3" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1370,8 +1371,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CY50"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2:Y45"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2:W45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17495,10 +17496,509 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25ABD3D7-7E41-464A-9ECA-BDE8895ACF15}">
+  <dimension ref="A1:C44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>167.91920399999998</v>
+      </c>
+      <c r="B1">
+        <v>236.69606200000001</v>
+      </c>
+      <c r="C1">
+        <v>101.51396100000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>168.50099999999998</v>
+      </c>
+      <c r="B2">
+        <v>166.71504300000001</v>
+      </c>
+      <c r="C2">
+        <v>170.22537199999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>71.615229000000014</v>
+      </c>
+      <c r="B3">
+        <v>54.190128000000016</v>
+      </c>
+      <c r="C3">
+        <v>88.439464000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>104.61701500000001</v>
+      </c>
+      <c r="B4">
+        <v>82.800314999999998</v>
+      </c>
+      <c r="C4">
+        <v>125.68141499999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>151.21848200000002</v>
+      </c>
+      <c r="B5">
+        <v>126.760766</v>
+      </c>
+      <c r="C5">
+        <v>174.83282800000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>143.37455600000001</v>
+      </c>
+      <c r="B6">
+        <v>140.911664</v>
+      </c>
+      <c r="C6">
+        <v>145.75252</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>162.35406700000001</v>
+      </c>
+      <c r="B7">
+        <v>130.175816</v>
+      </c>
+      <c r="C7">
+        <v>193.422721</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>171.996568</v>
+      </c>
+      <c r="B8">
+        <v>164.38618700000001</v>
+      </c>
+      <c r="C8">
+        <v>179.34452200000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>50.656300999999999</v>
+      </c>
+      <c r="B9">
+        <v>47.369717999999992</v>
+      </c>
+      <c r="C9">
+        <v>53.82955299999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>220.69427400000001</v>
+      </c>
+      <c r="B10">
+        <v>219.950884</v>
+      </c>
+      <c r="C10">
+        <v>221.41202899999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>26.378552000000013</v>
+      </c>
+      <c r="B11">
+        <v>-8.6589619999999954</v>
+      </c>
+      <c r="C11">
+        <v>60.207875999999942</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>45.195063000000005</v>
+      </c>
+      <c r="B12">
+        <v>31.872962999999999</v>
+      </c>
+      <c r="C12">
+        <v>58.057779999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>183.64984900000002</v>
+      </c>
+      <c r="B13">
+        <v>176.98636299999998</v>
+      </c>
+      <c r="C13">
+        <v>190.08355899999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>124.398298</v>
+      </c>
+      <c r="B14">
+        <v>116.63462299999999</v>
+      </c>
+      <c r="C14">
+        <v>131.89426</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>85.385324000000011</v>
+      </c>
+      <c r="B15">
+        <v>61.027045999999999</v>
+      </c>
+      <c r="C15">
+        <v>108.903665</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>160.734274</v>
+      </c>
+      <c r="B16">
+        <v>157.97506300000001</v>
+      </c>
+      <c r="C16">
+        <v>163.39833999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>141.80726799999999</v>
+      </c>
+      <c r="B17">
+        <v>142.756631</v>
+      </c>
+      <c r="C17">
+        <v>140.89064100000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>106.69883799999999</v>
+      </c>
+      <c r="B18">
+        <v>78.176758000000021</v>
+      </c>
+      <c r="C18">
+        <v>134.23739899999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>121.553439</v>
+      </c>
+      <c r="B19">
+        <v>163.61022500000001</v>
+      </c>
+      <c r="C19">
+        <v>80.946888999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>111.46267399999999</v>
+      </c>
+      <c r="B20">
+        <v>131.382992</v>
+      </c>
+      <c r="C20">
+        <v>92.229264000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>63.745367999999985</v>
+      </c>
+      <c r="B21">
+        <v>45.540071000000005</v>
+      </c>
+      <c r="C21">
+        <v>81.322893999999991</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>-15.778303999999991</v>
+      </c>
+      <c r="B22">
+        <v>-20.738235000000017</v>
+      </c>
+      <c r="C22">
+        <v>-10.989405000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>180.521061</v>
+      </c>
+      <c r="B23">
+        <v>228.909381</v>
+      </c>
+      <c r="C23">
+        <v>133.801301</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>107.62711999999999</v>
+      </c>
+      <c r="B24">
+        <v>126.37523399999999</v>
+      </c>
+      <c r="C24">
+        <v>89.525492999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>-33.582603999999989</v>
+      </c>
+      <c r="B25">
+        <v>-98.951114999999987</v>
+      </c>
+      <c r="C25">
+        <v>29.531819999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>68.069913</v>
+      </c>
+      <c r="B26">
+        <v>71.532898999999986</v>
+      </c>
+      <c r="C26">
+        <v>64.726340999999991</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>153.072337</v>
+      </c>
+      <c r="B27">
+        <v>178.08245400000001</v>
+      </c>
+      <c r="C27">
+        <v>128.92464000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>68.219248999999991</v>
+      </c>
+      <c r="B28">
+        <v>97.057412999999997</v>
+      </c>
+      <c r="C28">
+        <v>40.37550499999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>156.66850699999998</v>
+      </c>
+      <c r="B29">
+        <v>97.763801000000001</v>
+      </c>
+      <c r="C29">
+        <v>213.54201699999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>186.48440299999999</v>
+      </c>
+      <c r="B30">
+        <v>192.10031699999999</v>
+      </c>
+      <c r="C30">
+        <v>181.06214399999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>50.495852999999997</v>
+      </c>
+      <c r="B31">
+        <v>42.947164000000008</v>
+      </c>
+      <c r="C31">
+        <v>57.784244999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>140.94058999999999</v>
+      </c>
+      <c r="B32">
+        <v>118.31582200000001</v>
+      </c>
+      <c r="C32">
+        <v>162.78519200000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>145.51759899999999</v>
+      </c>
+      <c r="B33">
+        <v>135.09875199999999</v>
+      </c>
+      <c r="C33">
+        <v>155.57717500000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>183.74356400000002</v>
+      </c>
+      <c r="B34">
+        <v>141.48209499999999</v>
+      </c>
+      <c r="C34">
+        <v>224.54774200000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>120.42436199999999</v>
+      </c>
+      <c r="B35">
+        <v>123.48393799999998</v>
+      </c>
+      <c r="C35">
+        <v>117.47028800000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>86.134162000000003</v>
+      </c>
+      <c r="B36">
+        <v>139.43277700000002</v>
+      </c>
+      <c r="C36">
+        <v>34.673429999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>170.375181</v>
+      </c>
+      <c r="B37">
+        <v>173.05895100000001</v>
+      </c>
+      <c r="C37">
+        <v>167.78395499999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>143.201672</v>
+      </c>
+      <c r="B38">
+        <v>140.841733</v>
+      </c>
+      <c r="C38">
+        <v>145.480234</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>174.36840100000003</v>
+      </c>
+      <c r="B39">
+        <v>178.71554900000001</v>
+      </c>
+      <c r="C39">
+        <v>170.171155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>131.41501199999999</v>
+      </c>
+      <c r="B40">
+        <v>135.938197</v>
+      </c>
+      <c r="C40">
+        <v>127.047798</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>49.678787999999997</v>
+      </c>
+      <c r="B41">
+        <v>61.819854999999997</v>
+      </c>
+      <c r="C41">
+        <v>37.956377999999994</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>61.726566000000005</v>
+      </c>
+      <c r="B42">
+        <v>36.631985</v>
+      </c>
+      <c r="C42">
+        <v>85.955816999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>86.109937000000002</v>
+      </c>
+      <c r="B43">
+        <v>87.457910999999996</v>
+      </c>
+      <c r="C43">
+        <v>84.808447000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>188.93338199999999</v>
+      </c>
+      <c r="B44">
+        <v>195.98769200000001</v>
+      </c>
+      <c r="C44">
+        <v>182.12232600000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BACBDC8-A22A-414E-BCDA-165696315C70}">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -17993,7 +18493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E45"/>
   <sheetViews>
@@ -18773,7 +19273,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E45"/>
   <sheetViews>
@@ -19553,7 +20053,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E45"/>
   <sheetViews>
@@ -20333,7 +20833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E45"/>
   <sheetViews>
@@ -21113,7 +21613,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E45"/>
   <sheetViews>

</xml_diff>